<commit_message>
Actualizacion de las question del logcanal
</commit_message>
<xml_diff>
--- a/APP_PERSONAS_XML/src/test/resources/datadriven/tarjetadecredito/Trn_0533ConsultaCostoAvanceTarjeta.xlsx
+++ b/APP_PERSONAS_XML/src/test/resources/datadriven/tarjetadecredito/Trn_0533ConsultaCostoAvanceTarjeta.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
   <si>
     <t>orientacion</t>
   </si>
@@ -138,9 +138,6 @@
     <t>Depositos</t>
   </si>
   <si>
-    <t>0322</t>
-  </si>
-  <si>
     <t>TRANSACCION EXITOSA</t>
   </si>
   <si>
@@ -154,6 +151,15 @@
   </si>
   <si>
     <t>5303710222339850</t>
+  </si>
+  <si>
+    <t>0533</t>
+  </si>
+  <si>
+    <t>CUENTA NO AUTORIZADA A LA SOLICITUD</t>
+  </si>
+  <si>
+    <t>004</t>
   </si>
 </sst>
 </file>
@@ -560,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -608,10 +614,10 @@
         <v>3</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -640,16 +646,16 @@
         <v>5</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="K2" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -672,22 +678,22 @@
         <v>33</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:12">

</xml_diff>